<commit_message>
Re-running everything with 5,000 runs
Because difficult to manage with 10,000 even when decomposing
</commit_message>
<xml_diff>
--- a/output/sites/percent_differences_with_all_scat_est_all_scenarios_Cap Noir.xlsx
+++ b/output/sites/percent_differences_with_all_scat_est_all_scenarios_Cap Noir.xlsx
@@ -416,19 +416,19 @@
         <v>9</v>
       </c>
       <c r="C2" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>29</v>
       </c>
       <c r="G2" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H2" t="n">
         <v>31</v>
@@ -474,25 +474,25 @@
         <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D4" t="n">
         <v>29</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
         <v>23</v>
       </c>
       <c r="G4" t="n">
+        <v>23</v>
+      </c>
+      <c r="H4" t="n">
         <v>24</v>
       </c>
-      <c r="H4" t="n">
-        <v>25</v>
-      </c>
       <c r="I4" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
@@ -506,10 +506,10 @@
         <v>34</v>
       </c>
       <c r="D5" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>11</v>
@@ -538,16 +538,16 @@
         <v>-85</v>
       </c>
       <c r="E6" t="n">
-        <v>-14</v>
+        <v>-15</v>
       </c>
       <c r="F6" t="n">
-        <v>-24</v>
+        <v>-25</v>
       </c>
       <c r="G6" t="n">
-        <v>-69</v>
+        <v>-70</v>
       </c>
       <c r="H6" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="I6" t="n">
         <v>-89</v>
@@ -564,7 +564,7 @@
         <v>79</v>
       </c>
       <c r="D7" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" t="n">
         <v>9</v>
@@ -573,13 +573,13 @@
         <v>15</v>
       </c>
       <c r="G7" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H7" t="n">
         <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8">
@@ -634,7 +634,7 @@
         <v>-79</v>
       </c>
       <c r="H9" t="n">
-        <v>-19</v>
+        <v>-20</v>
       </c>
       <c r="I9" t="n">
         <v>-93</v>
@@ -651,16 +651,16 @@
         <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n">
         <v>71</v>
       </c>
       <c r="G10" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H10" t="n">
         <v>157</v>

</xml_diff>